<commit_message>
not completely broken but nlp breaking may constraints
</commit_message>
<xml_diff>
--- a/data/case9_DC.xlsx
+++ b/data/case9_DC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samho\Desktop\PhD\DC OPF\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D7320A-009D-47E0-AE32-E6CEE7D489B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F6DAB9-CD16-4205-BF0C-8AA05FA04E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ac_links" sheetId="12" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="126">
   <si>
     <t>name</t>
   </si>
@@ -411,6 +411,9 @@
   </si>
   <si>
     <t>MTDC</t>
+  </si>
+  <si>
+    <t>poles</t>
   </si>
 </sst>
 </file>
@@ -442,7 +445,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -465,13 +468,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -790,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2377B432-B755-4411-A970-729F4FF71B71}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1244,7 +1261,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G26" activeCellId="1" sqref="A5:F10 G26"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1679,10 +1696,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1690,7 +1707,7 @@
     <col min="1" max="1025" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1730,8 +1747,11 @@
       <c r="M1" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N1" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -1744,8 +1764,8 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
+      <c r="E2">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="F2" t="s">
         <v>49</v>
@@ -1771,8 +1791,11 @@
       <c r="M2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1812,8 +1835,11 @@
       <c r="M3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -1853,8 +1879,11 @@
       <c r="M4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -1867,8 +1896,8 @@
       <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
-        <v>13</v>
+      <c r="E5">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="F5" t="s">
         <v>64</v>
@@ -1894,8 +1923,11 @@
       <c r="M5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -1935,8 +1967,11 @@
       <c r="M6" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -1976,8 +2011,11 @@
       <c r="M7" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>74</v>
       </c>
@@ -1990,8 +2028,8 @@
       <c r="D8" t="s">
         <v>10</v>
       </c>
-      <c r="E8" t="s">
-        <v>13</v>
+      <c r="E8">
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="F8" t="s">
         <v>75</v>
@@ -2017,8 +2055,11 @@
       <c r="M8" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>76</v>
       </c>
@@ -2058,8 +2099,11 @@
       <c r="M9" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>80</v>
       </c>
@@ -2098,6 +2142,9 @@
       </c>
       <c r="M10" t="s">
         <v>53</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed nlp errors but now constraint issues
</commit_message>
<xml_diff>
--- a/data/case9_DC.xlsx
+++ b/data/case9_DC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samho\Desktop\PhD\DC OPF\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A89132-8DC0-48A3-A61C-1BFB960D51EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F77CD820-44BD-49B0-8F50-F91FC9778541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ac_links" sheetId="12" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="125">
   <si>
     <t>name</t>
   </si>
@@ -408,6 +408,9 @@
   </si>
   <si>
     <t>MTDC</t>
+  </si>
+  <si>
+    <t>poles</t>
   </si>
 </sst>
 </file>
@@ -439,7 +442,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -462,13 +465,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -787,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2377B432-B755-4411-A970-729F4FF71B71}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1688,10 +1705,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1699,7 +1716,7 @@
     <col min="1" max="1025" width="8.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1739,8 +1756,11 @@
       <c r="M1" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N1" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -1753,8 +1773,8 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
+      <c r="E2">
+        <v>9.9999999999999995E-8</v>
       </c>
       <c r="F2" t="s">
         <v>49</v>
@@ -1780,8 +1800,11 @@
       <c r="M2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1821,8 +1844,11 @@
       <c r="M3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -1862,8 +1888,11 @@
       <c r="M4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>63</v>
       </c>
@@ -1876,8 +1905,8 @@
       <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
-        <v>13</v>
+      <c r="E5">
+        <v>9.9999999999999995E-8</v>
       </c>
       <c r="F5" t="s">
         <v>64</v>
@@ -1903,8 +1932,11 @@
       <c r="M5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -1944,8 +1976,11 @@
       <c r="M6" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -1985,8 +2020,11 @@
       <c r="M7" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>74</v>
       </c>
@@ -1999,8 +2037,8 @@
       <c r="D8" t="s">
         <v>10</v>
       </c>
-      <c r="E8" t="s">
-        <v>13</v>
+      <c r="E8">
+        <v>9.9999999999999995E-8</v>
       </c>
       <c r="F8" t="s">
         <v>75</v>
@@ -2026,8 +2064,11 @@
       <c r="M8" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>76</v>
       </c>
@@ -2067,8 +2108,11 @@
       <c r="M9" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>80</v>
       </c>
@@ -2107,6 +2151,9 @@
       </c>
       <c r="M10" t="s">
         <v>53</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>